<commit_message>
Updating visualizations to have colorbars and multiaxis
</commit_message>
<xml_diff>
--- a/data_visualization/borough_pop.xlsx
+++ b/data_visualization/borough_pop.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>BROOKLYN</t>
   </si>
@@ -53,16 +53,10 @@
     <t>population</t>
   </si>
   <si>
-    <t>crimes per capita</t>
+    <t>Crimes per capita</t>
   </si>
   <si>
-    <t>pop / mi^2</t>
-  </si>
-  <si>
-    <t>norm crimes per capita</t>
-  </si>
-  <si>
-    <t>norm pop/mi^2</t>
+    <t>Population per square mile</t>
   </si>
 </sst>
 </file>
@@ -240,7 +234,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Normalized crimes per capita</c:v>
+            <c:strRef>
+              <c:f>crime_counts!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Crimes per capita</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -279,91 +281,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>crime_counts!$G$2:$G$6</c:f>
+              <c:f>crime_counts!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.487481208298744</c:v>
+                  <c:v>0.796698885574266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0579899331309605</c:v>
+                  <c:v>0.609339641474029</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.400804709609428</c:v>
+                  <c:v>0.766927112070134</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.512518791701256</c:v>
+                  <c:v>0.453217388809542</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.317777193075956</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Normalized population per square mile</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>crime_counts!$A$2:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>BRONX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>BROOKLYN</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MANHATTAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>QUEENS</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>STATEN ISLAND</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>crime_counts!$H$2:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-0.012033476942635</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0436508629244579</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.587577549083117</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.206772484148057</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.412422450916883</c:v>
+                  <c:v>0.520107524587716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,12 +313,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082692832"/>
-        <c:axId val="2140717152"/>
+        <c:axId val="-2079721968"/>
+        <c:axId val="-2080013792"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>crime_counts!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Population per square mile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>crime_counts!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32613.79797504121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36038.84892086331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69494.87291849254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20635.72617946346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7986.539444539104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2060306832"/>
+        <c:axId val="-2098178000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082692832"/>
+        <c:axId val="-2079721968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140717152"/>
+        <c:crossAx val="-2080013792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140717152"/>
+        <c:axId val="-2080013792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,10 +489,68 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082692832"/>
+        <c:crossAx val="-2079721968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="-2098178000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2060306832"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2060306832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2098178000"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1127,15 +1189,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
+      <xdr:colOff>615950</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1854200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1423,13 +1485,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1452,12 +1515,8 @@
       <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1480,14 +1539,6 @@
         <f>D2/C2</f>
         <v>32613.797975041205</v>
       </c>
-      <c r="G2">
-        <f>(E2-AVERAGE($E$2:$E$6))/(MAX($E$2:$E$6)-MIN($E$2:$E$6))</f>
-        <v>0.48748120829874358</v>
-      </c>
-      <c r="H2">
-        <f>(F2-AVERAGE($F$2:$F$6))/(MAX($F$2:$F$6)-MIN($F$2:$F$6))</f>
-        <v>-1.2033476942634964E-2</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1510,14 +1561,6 @@
         <f t="shared" ref="F3:F6" si="1">D3/C3</f>
         <v>36038.848920863311</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G6" si="2">(E3-AVERAGE($E$2:$E$6))/(MAX($E$2:$E$6)-MIN($E$2:$E$6))</f>
-        <v>-5.7989933130960535E-2</v>
-      </c>
-      <c r="H3">
-        <f>(F3-AVERAGE($F$2:$F$6))/(MAX($F$2:$F$6)-MIN($F$2:$F$6))</f>
-        <v>4.3650862924457863E-2</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1540,14 +1583,6 @@
         <f t="shared" si="1"/>
         <v>69494.872918492547</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
-        <v>0.40080470960942849</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H6" si="3">(F4-AVERAGE($F$2:$F$6))/(MAX($F$2:$F$6)-MIN($F$2:$F$6))</f>
-        <v>0.58757754908311721</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1570,14 +1605,6 @@
         <f t="shared" si="1"/>
         <v>20635.726179463461</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>-0.51251879170125647</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="3"/>
-        <v>-0.20677248414805738</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1599,14 +1626,6 @@
       <c r="F6">
         <f t="shared" si="1"/>
         <v>7986.5394445391039</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>-0.31777719307595559</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="3"/>
-        <v>-0.41242245091688284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Excel workbooks to have axises
</commit_message>
<xml_diff>
--- a/data_visualization/borough_pop.xlsx
+++ b/data_visualization/borough_pop.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="crime_counts" sheetId="1" r:id="rId1"/>
@@ -315,8 +315,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2079721968"/>
-        <c:axId val="-2080013792"/>
+        <c:axId val="2127970080"/>
+        <c:axId val="2127973440"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -383,11 +383,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2060306832"/>
-        <c:axId val="-2098178000"/>
+        <c:axId val="2127980224"/>
+        <c:axId val="2127977024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2079721968"/>
+        <c:axId val="2127970080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080013792"/>
+        <c:crossAx val="2127973440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -438,7 +438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080013792"/>
+        <c:axId val="2127973440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,6 +458,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Crimes per capita (crimes/population)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -489,17 +545,78 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079721968"/>
+        <c:crossAx val="2127970080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098178000"/>
+        <c:axId val="2127977024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Population</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> density (population/mi^2)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -531,12 +648,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2060306832"/>
+        <c:crossAx val="2127980224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2060306832"/>
+        <c:axId val="2127980224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +662,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098178000"/>
+        <c:crossAx val="2127977024"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1485,7 +1603,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>